<commit_message>
Tested and evaluated piezo sensors
</commit_message>
<xml_diff>
--- a/Elektronik/2017/Stückliste.xlsx
+++ b/Elektronik/2017/Stückliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>http://ch.farnell.com/multicomp/usb-b-s-ra/usb-2-0-buchse-typ-b-tht/dp/2112373?MER=sy-me-pd-mi-alte</t>
+  </si>
+  <si>
+    <t>2 Pins</t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,6 +1128,23 @@
         <v>103</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
@@ -1151,6 +1171,9 @@
       <c r="D29" t="s">
         <v>70</v>
       </c>
+      <c r="E29">
+        <v>0.378</v>
+      </c>
       <c r="F29" s="4" t="s">
         <v>64</v>
       </c>
@@ -1165,6 +1188,9 @@
       <c r="D30" t="s">
         <v>71</v>
       </c>
+      <c r="E30">
+        <v>0.25919999999999999</v>
+      </c>
       <c r="F30" s="4" t="s">
         <v>65</v>
       </c>
@@ -1179,6 +1205,9 @@
       <c r="D31" t="s">
         <v>72</v>
       </c>
+      <c r="E31">
+        <v>0.50760000000000005</v>
+      </c>
       <c r="F31" s="4" t="s">
         <v>66</v>
       </c>
@@ -1193,6 +1222,9 @@
       <c r="D32" t="s">
         <v>73</v>
       </c>
+      <c r="E32">
+        <v>1.22</v>
+      </c>
       <c r="F32" s="4" t="s">
         <v>67</v>
       </c>
@@ -1207,6 +1239,9 @@
       <c r="D33" t="s">
         <v>74</v>
       </c>
+      <c r="E33">
+        <v>0.97199999999999998</v>
+      </c>
       <c r="F33" s="4" t="s">
         <v>104</v>
       </c>
@@ -1221,6 +1256,9 @@
       <c r="D34" t="s">
         <v>75</v>
       </c>
+      <c r="E34">
+        <v>0.69120000000000004</v>
+      </c>
       <c r="F34" s="4" t="s">
         <v>68</v>
       </c>
@@ -1234,6 +1272,9 @@
       </c>
       <c r="D35" t="s">
         <v>76</v>
+      </c>
+      <c r="E35">
+        <v>1.3</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>69</v>
@@ -1260,9 +1301,11 @@
     <hyperlink ref="F18" r:id="rId17"/>
     <hyperlink ref="F19" r:id="rId18"/>
     <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F33" r:id="rId20"/>
+    <hyperlink ref="F21" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>